<commit_message>
fix: Bombs weren't despawning
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>l7</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
@@ -674,6 +680,69 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E3FC53-DF6F-45BF-A277-ACA82C20E2D9}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>2084.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>2605.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F06A1B3-4662-4CB9-A146-4F17B36F623F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -695,7 +764,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -703,23 +772,23 @@
         <v>2</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>521.0</v>
+        <v>2605.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>2084.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>1042.0</v>
+        <v>1563.0</v>
       </c>
     </row>
   </sheetData>
@@ -727,48 +796,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F06A1B3-4662-4CB9-A146-4F17B36F623F}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>2605.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6348C88F-41BF-45E4-838C-56BA43C0AFD0}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -808,6 +838,22 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>4168.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Added Rules Screen
Start screen has a rules button that take them to a screen that displays the rules to the player.
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>l</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -429,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -593,6 +602,14 @@
       </c>
       <c r="B20" t="n" s="0">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B21" t="n" s="0">
+        <v>1042.0</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +658,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98060BC9-2618-4D68-A88C-007ABEB60946}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -671,6 +688,30 @@
       </c>
       <c r="B3" t="n" s="0">
         <v>521.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>3126.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>3126.0</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +784,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F06A1B3-4662-4CB9-A146-4F17B36F623F}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -789,6 +830,14 @@
       </c>
       <c r="B5" t="n" s="0">
         <v>1563.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>2084.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style: Restyled start screen
Start screen was too clustered so I changed it to look less clustered.
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -610,6 +616,102 @@
       </c>
       <c r="B21" t="n" s="0">
         <v>1042.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B22" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n" s="0">
+        <v>1563.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B25" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B26" t="n" s="0">
+        <v>4168.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B27" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B28" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B29" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B30" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B31" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B32" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B33" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +823,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E3FC53-DF6F-45BF-A277-ACA82C20E2D9}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -777,6 +879,30 @@
         <v>2605.0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -784,7 +910,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F06A1B3-4662-4CB9-A146-4F17B36F623F}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -838,6 +964,14 @@
       </c>
       <c r="B6" t="n" s="0">
         <v>2084.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>16151.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added levels to the game
Added 3 levels, 1 being the easiest, and 3 the hardest which change the speed of the snake.
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>q</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -712,6 +715,430 @@
       </c>
       <c r="B33" t="n" s="0">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B34" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B35" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B36" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B37" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B38" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B40" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B41" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B42" t="n" s="0">
+        <v>1563.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B43" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B44" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B45" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B46" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B48" t="n" s="0">
+        <v>4689.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B50" t="n" s="0">
+        <v>2084.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B51" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B52" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B53" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B54" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B56" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B57" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B58" t="n" s="0">
+        <v>1563.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B59" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B60" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B61" t="n" s="0">
+        <v>5210.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B62" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B63" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B64" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B65" t="n" s="0">
+        <v>3647.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B66" t="n" s="0">
+        <v>2084.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B67" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B68" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B69" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B70" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B71" t="n" s="0">
+        <v>1563.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B72" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B73" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B74" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B75" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B76" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B77" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B78" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B79" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B80" t="n" s="0">
+        <v>2605.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B81" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B82" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B83" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B84" t="n" s="0">
+        <v>3126.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B85" t="n" s="0">
+        <v>1563.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B86" t="n" s="0">
+        <v>2605.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: 'Cleaned' up code in Application Package
Removed any unused variables and imports. Also simplified some lambda expressions.
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Resources/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -447,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1139,6 +1139,22 @@
       </c>
       <c r="B86" t="n" s="0">
         <v>2605.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B87" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B88" t="n" s="0">
+        <v>4168.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>